<commit_message>
Some User stories added
</commit_message>
<xml_diff>
--- a/TeamWeeklyReport_TEAM1.xlsx
+++ b/TeamWeeklyReport_TEAM1.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcb0033\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l3ryc\Documents\School\College\CS 499\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747101DE-1431-4946-861D-226129EB7755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{8166B2E4-7435-44CF-B2CE-A0D05147DBA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Members List" sheetId="1" r:id="rId1"/>
@@ -26,7 +28,7 @@
     <sheet name="Problem Reports" sheetId="12" r:id="rId12"/>
     <sheet name="Lists" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -102,12 +104,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -121,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -135,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -154,12 +156,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -172,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -186,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -204,12 +206,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -227,12 +229,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -259,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -272,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -291,12 +293,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -315,12 +317,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -338,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="406">
   <si>
     <t>Name</t>
   </si>
@@ -1502,12 +1504,66 @@
   </si>
   <si>
     <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Truth Table Construction</t>
+  </si>
+  <si>
+    <t>Construct Truth Table from wff. Note any tautologies or contradictions.</t>
+  </si>
+  <si>
+    <t>Tautological Proofing</t>
+  </si>
+  <si>
+    <t>Convert left side of bioconditional statement to right side in order to verify a tautology. Step-by-step justification required.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 1.1 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 1.2 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 3.1 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 4.1 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 5.1 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 5.4 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 5.5 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 5.7 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 6.1 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 6.2 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to review Problems from Section 7.1 so that I can see their solutions and a step-by-step guide to solving them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 1.1 Web-Examples </t>
+  </si>
+  <si>
+    <t>Lay out example problems from Section 1.1 on web</t>
+  </si>
+  <si>
+    <t>Justify Proofing Sequence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
@@ -1807,14 +1863,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5001,10 +5058,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5012,13 +5069,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$9</xm:f>
           </x14:formula1>
@@ -5031,11 +5088,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6119,11 +6177,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7225,13 +7284,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$F$2:$F$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
           <x14:formula1>
             <xm:f>'Members List'!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -7244,11 +7303,12 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8505,13 +8565,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$G$2:$G$5</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
           <x14:formula1>
             <xm:f>'Members List'!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -8524,7 +8584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
@@ -8532,6 +8592,7 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9704,7 +9765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
@@ -9714,6 +9775,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11018,7 +11080,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$B$2:$B$6</xm:f>
           </x14:formula1>
@@ -11031,14 +11093,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12252,19 +12315,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$5</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>'Members List'!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="date" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="date" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>Lists!D2</xm:f>
           </x14:formula1>
@@ -12280,13 +12343,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12350,7 +12416,7 @@
         <v>356</v>
       </c>
       <c r="C3" t="s">
-        <v>369</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -12372,7 +12438,7 @@
         <v>372</v>
       </c>
       <c r="C5" t="s">
-        <v>374</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -12394,7 +12460,7 @@
         <v>357</v>
       </c>
       <c r="C7" t="s">
-        <v>375</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -12416,7 +12482,7 @@
         <v>358</v>
       </c>
       <c r="C9" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -12438,7 +12504,7 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>377</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -12460,7 +12526,7 @@
         <v>360</v>
       </c>
       <c r="C13" t="s">
-        <v>378</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -12482,7 +12548,7 @@
         <v>361</v>
       </c>
       <c r="C15" t="s">
-        <v>379</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12504,7 +12570,7 @@
         <v>362</v>
       </c>
       <c r="C17" t="s">
-        <v>380</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12526,7 +12592,7 @@
         <v>363</v>
       </c>
       <c r="C19" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12548,7 +12614,7 @@
         <v>364</v>
       </c>
       <c r="C21" t="s">
-        <v>382</v>
+        <v>401</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12570,7 +12636,7 @@
         <v>365</v>
       </c>
       <c r="C23" t="s">
-        <v>383</v>
+        <v>402</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13588,13 +13654,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13651,25 +13720,59 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="C2" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="2"/>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="C3" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" s="2"/>
+      <c r="G3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>404</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -13678,6 +13781,9 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>84</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>405</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -14854,22 +14960,28 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>'Members List'!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>E2:F30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>Epics!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A30</xm:sqref>
+          <xm:sqref>A3:A30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{381C3F0C-3DAB-41B1-AD7D-E3EB678F27CA}">
+          <x14:formula1>
+            <xm:f>Epics!$A$2:$A$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14878,11 +14990,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15958,13 +16071,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17226,13 +17340,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>'Configuration Items'!$A$2:$A$11</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A35</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>'Members List'!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -17245,11 +17359,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18309,7 +18424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
@@ -18317,6 +18432,7 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19867,7 +19983,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$H$2:$H$9</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
start of recusion from a few days ago
</commit_message>
<xml_diff>
--- a/TeamWeeklyReport_TEAM1.xlsx
+++ b/TeamWeeklyReport_TEAM1.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l3ryc\Documents\School\College\CS 499\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\OneDrive\Desktop\CS-499\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747101DE-1431-4946-861D-226129EB7755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7424DCA3-78F3-4023-9EFE-B9D5F4D4074E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{8166B2E4-7435-44CF-B2CE-A0D05147DBA2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5805" yWindow="3735" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="2" xr2:uid="{8166B2E4-7435-44CF-B2CE-A0D05147DBA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Members List" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,14 @@
     <sheet name="Problem Reports" sheetId="12" r:id="rId12"/>
     <sheet name="Lists" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -54,6 +56,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Optional </t>
@@ -67,6 +70,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Use the Class cells to enter current student class schedule for the term. </t>
@@ -80,6 +84,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Enter student work schedule. </t>
@@ -93,6 +98,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Other scheduled items such as other meetings or commitments that need to be taken in account. </t>
@@ -116,6 +122,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Copied from Members List
@@ -130,6 +137,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Select Role or Attendance
@@ -144,6 +152,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 If you team is keep meeting minutes in Word documents (or simular) attach the file here. 
@@ -168,6 +177,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Provide short title to help quickly identify the nature of the action. </t>
@@ -181,6 +191,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Details on what this action involves and relationships with other actions for tasks. 
@@ -195,6 +206,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Kevin Preston:
 How was the action resolved? Did the team agree with the closure information? Were other actions assigned because of this AI?</t>
@@ -218,6 +230,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Kevin Preston:
 Only use if your team is doing Epics and User Stories as part of Agile</t>
@@ -241,6 +254,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Only use if your team is doing Epics and User Stories as part of Agil
@@ -255,6 +269,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Kevin Preston:
 Short Title</t>
@@ -268,6 +283,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Full User Story in the required format. </t>
@@ -281,6 +297,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Which team member is assigned to implement this user Story. 
@@ -305,6 +322,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Mitigation Steps should be put on the Schedule Tab.
@@ -329,6 +347,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kevin Preston:
 Owner has performed the action but the team has to agee to the closure plan. </t>
@@ -1578,17 +1597,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11101,7 +11123,9 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12352,7 +12376,7 @@
       <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13660,10 +13684,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>